<commit_message>
Added inventory item code for generic access to inventoy
</commit_message>
<xml_diff>
--- a/Ultima5Redux/Data/U5SupplementaryWorkbook.xlsx
+++ b/Ultima5Redux/Data/U5SupplementaryWorkbook.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Custom Signs" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,6 +21,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>New Magincia</t>
+  </si>
+  <si>
+    <t>Rushin\n1/1/136</t>
+  </si>
+  <si>
+    <t>8lllllllllllll9g   Òõóèéî    gg   ±¯±¯±³¶   gjlllllllllllllk</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -336,12 +350,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>